<commit_message>
Uploaded different worksheets, scripts and other stuff.
</commit_message>
<xml_diff>
--- a/BGY 16/04_Material/20180831 - BankAngebot.xlsx
+++ b/BGY 16/04_Material/20180831 - BankAngebot.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carso\Documents\bbs1\BGY 16\04_Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EBF3B01-5B12-426F-92C3-C11F90835244}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A14D520B-01AA-4D04-B4D3-74911757FB8A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12% Bank" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,14 +106,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -429,33 +429,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -543,7 +543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -553,20 +553,20 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -583,11 +583,11 @@
         <v>0.5</v>
       </c>
       <c r="B4">
-        <f>C3*0.06</f>
+        <f t="shared" ref="B4:B13" si="0">C3*0.06</f>
         <v>6</v>
       </c>
       <c r="C4">
-        <f>C3+B4</f>
+        <f t="shared" ref="C4:C13" si="1">C3+B4</f>
         <v>106</v>
       </c>
     </row>
@@ -596,11 +596,11 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <f>C4*0.06</f>
+        <f t="shared" si="0"/>
         <v>6.3599999999999994</v>
       </c>
       <c r="C5">
-        <f>C4+B5</f>
+        <f t="shared" si="1"/>
         <v>112.36</v>
       </c>
     </row>
@@ -609,11 +609,11 @@
         <v>1.5</v>
       </c>
       <c r="B6">
-        <f>C5*0.06</f>
+        <f t="shared" si="0"/>
         <v>6.7416</v>
       </c>
       <c r="C6">
-        <f>C5+B6</f>
+        <f t="shared" si="1"/>
         <v>119.1016</v>
       </c>
     </row>
@@ -622,11 +622,11 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <f>C6*0.06</f>
+        <f t="shared" si="0"/>
         <v>7.146096</v>
       </c>
       <c r="C7">
-        <f>C6+B7</f>
+        <f t="shared" si="1"/>
         <v>126.247696</v>
       </c>
     </row>
@@ -635,11 +635,11 @@
         <v>2.5</v>
       </c>
       <c r="B8">
-        <f>C7*0.06</f>
+        <f t="shared" si="0"/>
         <v>7.5748617600000001</v>
       </c>
       <c r="C8">
-        <f>C7+B8</f>
+        <f t="shared" si="1"/>
         <v>133.82255776</v>
       </c>
     </row>
@@ -648,11 +648,11 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <f>C8*0.06</f>
+        <f t="shared" si="0"/>
         <v>8.0293534655999999</v>
       </c>
       <c r="C9">
-        <f>C8+B9</f>
+        <f t="shared" si="1"/>
         <v>141.85191122559999</v>
       </c>
     </row>
@@ -661,11 +661,11 @@
         <v>3.5</v>
       </c>
       <c r="B10">
-        <f>C9*0.06</f>
+        <f t="shared" si="0"/>
         <v>8.5111146735359995</v>
       </c>
       <c r="C10">
-        <f>C9+B10</f>
+        <f t="shared" si="1"/>
         <v>150.36302589913601</v>
       </c>
     </row>
@@ -674,11 +674,11 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <f>C10*0.06</f>
+        <f t="shared" si="0"/>
         <v>9.0217815539481592</v>
       </c>
       <c r="C11">
-        <f>C10+B11</f>
+        <f t="shared" si="1"/>
         <v>159.38480745308416</v>
       </c>
     </row>
@@ -687,11 +687,11 @@
         <v>4.5</v>
       </c>
       <c r="B12">
-        <f>C11*0.06</f>
+        <f t="shared" si="0"/>
         <v>9.5630884471850504</v>
       </c>
       <c r="C12">
-        <f>C11+B12</f>
+        <f t="shared" si="1"/>
         <v>168.9478959002692</v>
       </c>
     </row>
@@ -700,11 +700,11 @@
         <v>5</v>
       </c>
       <c r="B13">
-        <f>C12*0.06</f>
+        <f t="shared" si="0"/>
         <v>10.136873754016152</v>
       </c>
       <c r="C13">
-        <f>C12+B13</f>
+        <f t="shared" si="1"/>
         <v>179.08476965428537</v>
       </c>
     </row>
@@ -717,30 +717,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1021,30 +1021,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C63"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1057,15 +1057,15 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="B4">
-        <f>C3*0.01</f>
+        <f t="shared" ref="B4:B35" si="0">C3*0.01</f>
         <v>1</v>
       </c>
       <c r="C4">
-        <f>C3+B4</f>
+        <f t="shared" ref="C4:C35" si="1">C3+B4</f>
         <v>101</v>
       </c>
     </row>
@@ -1074,24 +1074,24 @@
         <v>0.16666666666666699</v>
       </c>
       <c r="B5">
-        <f>C4*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.01</v>
       </c>
       <c r="C5">
-        <f>C4+B5</f>
+        <f t="shared" si="1"/>
         <v>102.01</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>0.25</v>
       </c>
       <c r="B6">
-        <f>C5*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.0201</v>
       </c>
       <c r="C6">
-        <f>C5+B6</f>
+        <f t="shared" si="1"/>
         <v>103.0301</v>
       </c>
     </row>
@@ -1100,24 +1100,24 @@
         <v>0.33333333333333298</v>
       </c>
       <c r="B7">
-        <f>C6*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.0303010000000001</v>
       </c>
       <c r="C7">
-        <f>C6+B7</f>
+        <f t="shared" si="1"/>
         <v>104.060401</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>0.41666666666666702</v>
       </c>
       <c r="B8">
-        <f>C7*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.04060401</v>
       </c>
       <c r="C8">
-        <f>C7+B8</f>
+        <f t="shared" si="1"/>
         <v>105.10100500999999</v>
       </c>
     </row>
@@ -1126,24 +1126,24 @@
         <v>0.5</v>
       </c>
       <c r="B9">
-        <f>C8*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.0510100500999999</v>
       </c>
       <c r="C9">
-        <f>C8+B9</f>
+        <f t="shared" si="1"/>
         <v>106.1520150601</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>0.58333333333333304</v>
       </c>
       <c r="B10">
-        <f>C9*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.0615201506009999</v>
       </c>
       <c r="C10">
-        <f>C9+B10</f>
+        <f t="shared" si="1"/>
         <v>107.213535210701</v>
       </c>
     </row>
@@ -1152,24 +1152,24 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B11">
-        <f>C10*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.0721353521070101</v>
       </c>
       <c r="C11">
-        <f>C10+B11</f>
+        <f t="shared" si="1"/>
         <v>108.28567056280801</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>0.75</v>
       </c>
       <c r="B12">
-        <f>C11*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.08285670562808</v>
       </c>
       <c r="C12">
-        <f>C11+B12</f>
+        <f t="shared" si="1"/>
         <v>109.36852726843608</v>
       </c>
     </row>
@@ -1178,24 +1178,24 @@
         <v>0.83333333333333304</v>
       </c>
       <c r="B13">
-        <f>C12*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.0936852726843609</v>
       </c>
       <c r="C13">
-        <f>C12+B13</f>
+        <f t="shared" si="1"/>
         <v>110.46221254112044</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>0.91666666666666696</v>
       </c>
       <c r="B14">
-        <f>C13*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.1046221254112043</v>
       </c>
       <c r="C14">
-        <f>C13+B14</f>
+        <f t="shared" si="1"/>
         <v>111.56683466653165</v>
       </c>
     </row>
@@ -1204,24 +1204,24 @@
         <v>1</v>
       </c>
       <c r="B15">
-        <f>C14*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.1156683466653166</v>
       </c>
       <c r="C15">
-        <f>C14+B15</f>
+        <f t="shared" si="1"/>
         <v>112.68250301319696</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>1.0833333333333299</v>
       </c>
       <c r="B16">
-        <f>C15*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.1268250301319698</v>
       </c>
       <c r="C16">
-        <f>C15+B16</f>
+        <f t="shared" si="1"/>
         <v>113.80932804332893</v>
       </c>
     </row>
@@ -1230,24 +1230,24 @@
         <v>1.1666666666666701</v>
       </c>
       <c r="B17">
-        <f>C16*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.1380932804332893</v>
       </c>
       <c r="C17">
-        <f>C16+B17</f>
+        <f t="shared" si="1"/>
         <v>114.94742132376223</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>1.25</v>
       </c>
       <c r="B18">
-        <f>C17*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.1494742132376223</v>
       </c>
       <c r="C18">
-        <f>C17+B18</f>
+        <f t="shared" si="1"/>
         <v>116.09689553699985</v>
       </c>
     </row>
@@ -1256,24 +1256,24 @@
         <v>1.3333333333333299</v>
       </c>
       <c r="B19">
-        <f>C18*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.1609689553699984</v>
       </c>
       <c r="C19">
-        <f>C18+B19</f>
+        <f t="shared" si="1"/>
         <v>117.25786449236985</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>1.4166666666666701</v>
       </c>
       <c r="B20">
-        <f>C19*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.1725786449236986</v>
       </c>
       <c r="C20">
-        <f>C19+B20</f>
+        <f t="shared" si="1"/>
         <v>118.43044313729355</v>
       </c>
     </row>
@@ -1282,24 +1282,24 @@
         <v>1.5</v>
       </c>
       <c r="B21">
-        <f>C20*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.1843044313729356</v>
       </c>
       <c r="C21">
-        <f>C20+B21</f>
+        <f t="shared" si="1"/>
         <v>119.61474756866649</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>1.5833333333333299</v>
       </c>
       <c r="B22">
-        <f>C21*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.1961474756866648</v>
       </c>
       <c r="C22">
-        <f>C21+B22</f>
+        <f t="shared" si="1"/>
         <v>120.81089504435315</v>
       </c>
     </row>
@@ -1308,24 +1308,24 @@
         <v>1.6666666666666701</v>
       </c>
       <c r="B23">
-        <f>C22*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.2081089504435314</v>
       </c>
       <c r="C23">
-        <f>C22+B23</f>
+        <f t="shared" si="1"/>
         <v>122.01900399479668</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>1.75</v>
       </c>
       <c r="B24">
-        <f>C23*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.2201900399479668</v>
       </c>
       <c r="C24">
-        <f>C23+B24</f>
+        <f t="shared" si="1"/>
         <v>123.23919403474464</v>
       </c>
     </row>
@@ -1334,24 +1334,24 @@
         <v>1.8333333333333299</v>
       </c>
       <c r="B25">
-        <f>C24*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.2323919403474464</v>
       </c>
       <c r="C25">
-        <f>C24+B25</f>
+        <f t="shared" si="1"/>
         <v>124.47158597509208</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>1.9166666666666701</v>
       </c>
       <c r="B26">
-        <f>C25*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.2447158597509209</v>
       </c>
       <c r="C26">
-        <f>C25+B26</f>
+        <f t="shared" si="1"/>
         <v>125.71630183484301</v>
       </c>
     </row>
@@ -1360,24 +1360,24 @@
         <v>2</v>
       </c>
       <c r="B27">
-        <f>C26*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.2571630183484301</v>
       </c>
       <c r="C27">
-        <f>C26+B27</f>
+        <f t="shared" si="1"/>
         <v>126.97346485319144</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>2.0833333333333299</v>
       </c>
       <c r="B28">
-        <f>C27*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.2697346485319145</v>
       </c>
       <c r="C28">
-        <f>C27+B28</f>
+        <f t="shared" si="1"/>
         <v>128.24319950172335</v>
       </c>
     </row>
@@ -1386,24 +1386,24 @@
         <v>2.1666666666666701</v>
       </c>
       <c r="B29">
-        <f>C28*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.2824319950172336</v>
       </c>
       <c r="C29">
-        <f>C28+B29</f>
+        <f t="shared" si="1"/>
         <v>129.52563149674057</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>2.25</v>
       </c>
       <c r="B30">
-        <f>C29*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.2952563149674057</v>
       </c>
       <c r="C30">
-        <f>C29+B30</f>
+        <f t="shared" si="1"/>
         <v>130.82088781170799</v>
       </c>
     </row>
@@ -1412,24 +1412,24 @@
         <v>2.3333333333333299</v>
       </c>
       <c r="B31">
-        <f>C30*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.30820887811708</v>
       </c>
       <c r="C31">
-        <f>C30+B31</f>
+        <f t="shared" si="1"/>
         <v>132.12909668982508</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>2.4166666666666701</v>
       </c>
       <c r="B32">
-        <f>C31*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.3212909668982509</v>
       </c>
       <c r="C32">
-        <f>C31+B32</f>
+        <f t="shared" si="1"/>
         <v>133.45038765672334</v>
       </c>
     </row>
@@ -1438,24 +1438,24 @@
         <v>2.5</v>
       </c>
       <c r="B33">
-        <f>C32*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.3345038765672335</v>
       </c>
       <c r="C33">
-        <f>C32+B33</f>
+        <f t="shared" si="1"/>
         <v>134.78489153329056</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>2.5833333333333299</v>
       </c>
       <c r="B34">
-        <f>C33*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.3478489153329056</v>
       </c>
       <c r="C34">
-        <f>C33+B34</f>
+        <f t="shared" si="1"/>
         <v>136.13274044862348</v>
       </c>
     </row>
@@ -1464,24 +1464,24 @@
         <v>2.6666666666666701</v>
       </c>
       <c r="B35">
-        <f>C34*0.01</f>
+        <f t="shared" si="0"/>
         <v>1.3613274044862349</v>
       </c>
       <c r="C35">
-        <f>C34+B35</f>
+        <f t="shared" si="1"/>
         <v>137.49406785310973</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>2.75</v>
       </c>
       <c r="B36">
-        <f>C35*0.01</f>
+        <f t="shared" ref="B36:B101" si="2">C35*0.01</f>
         <v>1.3749406785310974</v>
       </c>
       <c r="C36">
-        <f>C35+B36</f>
+        <f t="shared" ref="C36:C67" si="3">C35+B36</f>
         <v>138.86900853164082</v>
       </c>
     </row>
@@ -1490,24 +1490,24 @@
         <v>2.8333333333333299</v>
       </c>
       <c r="B37">
-        <f>C36*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.3886900853164081</v>
       </c>
       <c r="C37">
-        <f>C36+B37</f>
+        <f t="shared" si="3"/>
         <v>140.25769861695721</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <v>2.9166666666666701</v>
       </c>
       <c r="B38">
-        <f>C37*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.4025769861695723</v>
       </c>
       <c r="C38">
-        <f>C37+B38</f>
+        <f t="shared" si="3"/>
         <v>141.66027560312679</v>
       </c>
     </row>
@@ -1516,24 +1516,24 @@
         <v>3</v>
       </c>
       <c r="B39">
-        <f>C38*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.416602756031268</v>
       </c>
       <c r="C39">
-        <f>C38+B39</f>
+        <f t="shared" si="3"/>
         <v>143.07687835915806</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="2">
+      <c r="A40" s="1">
         <v>3.0833333333333299</v>
       </c>
       <c r="B40">
-        <f>C39*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.4307687835915806</v>
       </c>
       <c r="C40">
-        <f>C39+B40</f>
+        <f t="shared" si="3"/>
         <v>144.50764714274965</v>
       </c>
     </row>
@@ -1542,24 +1542,24 @@
         <v>3.1666666666666701</v>
       </c>
       <c r="B41">
-        <f>C40*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.4450764714274964</v>
       </c>
       <c r="C41">
-        <f>C40+B41</f>
+        <f t="shared" si="3"/>
         <v>145.95272361417713</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="2">
+      <c r="A42" s="1">
         <v>3.25</v>
       </c>
       <c r="B42">
-        <f>C41*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.4595272361417713</v>
       </c>
       <c r="C42">
-        <f>C41+B42</f>
+        <f t="shared" si="3"/>
         <v>147.41225085031891</v>
       </c>
     </row>
@@ -1568,24 +1568,24 @@
         <v>3.3333333333333299</v>
       </c>
       <c r="B43">
-        <f>C42*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.474122508503189</v>
       </c>
       <c r="C43">
-        <f>C42+B43</f>
+        <f t="shared" si="3"/>
         <v>148.88637335882211</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>3.4166666666666701</v>
       </c>
       <c r="B44">
-        <f>C43*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.4888637335882211</v>
       </c>
       <c r="C44">
-        <f>C43+B44</f>
+        <f t="shared" si="3"/>
         <v>150.37523709241034</v>
       </c>
     </row>
@@ -1594,24 +1594,24 @@
         <v>3.5</v>
       </c>
       <c r="B45">
-        <f>C44*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.5037523709241034</v>
       </c>
       <c r="C45">
-        <f>C44+B45</f>
+        <f t="shared" si="3"/>
         <v>151.87898946333445</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="2">
+      <c r="A46" s="1">
         <v>3.5833333333333299</v>
       </c>
       <c r="B46">
-        <f>C45*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.5187898946333445</v>
       </c>
       <c r="C46">
-        <f>C45+B46</f>
+        <f t="shared" si="3"/>
         <v>153.39777935796781</v>
       </c>
     </row>
@@ -1620,24 +1620,24 @@
         <v>3.6666666666666701</v>
       </c>
       <c r="B47">
-        <f>C46*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.5339777935796781</v>
       </c>
       <c r="C47">
-        <f>C46+B47</f>
+        <f t="shared" si="3"/>
         <v>154.93175715154749</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="2">
+      <c r="A48" s="1">
         <v>3.75</v>
       </c>
       <c r="B48">
-        <f>C47*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.549317571515475</v>
       </c>
       <c r="C48">
-        <f>C47+B48</f>
+        <f t="shared" si="3"/>
         <v>156.48107472306296</v>
       </c>
     </row>
@@ -1646,24 +1646,24 @@
         <v>3.8333333333333299</v>
       </c>
       <c r="B49">
-        <f>C48*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.5648107472306296</v>
       </c>
       <c r="C49">
-        <f>C48+B49</f>
+        <f t="shared" si="3"/>
         <v>158.0458854702936</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>3.9166666666666701</v>
       </c>
       <c r="B50">
-        <f>C49*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.5804588547029361</v>
       </c>
       <c r="C50">
-        <f>C49+B50</f>
+        <f t="shared" si="3"/>
         <v>159.62634432499652</v>
       </c>
     </row>
@@ -1672,24 +1672,24 @@
         <v>4</v>
       </c>
       <c r="B51">
-        <f>C50*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.5962634432499652</v>
       </c>
       <c r="C51">
-        <f>C50+B51</f>
+        <f t="shared" si="3"/>
         <v>161.22260776824649</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="2">
+      <c r="A52" s="1">
         <v>4.0833333333333304</v>
       </c>
       <c r="B52">
-        <f>C51*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.6122260776824648</v>
       </c>
       <c r="C52">
-        <f>C51+B52</f>
+        <f t="shared" si="3"/>
         <v>162.83483384592896</v>
       </c>
     </row>
@@ -1698,24 +1698,24 @@
         <v>4.1666666666666696</v>
       </c>
       <c r="B53">
-        <f>C52*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.6283483384592896</v>
       </c>
       <c r="C53">
-        <f>C52+B53</f>
+        <f t="shared" si="3"/>
         <v>164.46318218438824</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="2">
+      <c r="A54" s="1">
         <v>4.25</v>
       </c>
       <c r="B54">
-        <f>C53*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.6446318218438825</v>
       </c>
       <c r="C54">
-        <f>C53+B54</f>
+        <f t="shared" si="3"/>
         <v>166.10781400623213</v>
       </c>
     </row>
@@ -1724,24 +1724,24 @@
         <v>4.3333333333333304</v>
       </c>
       <c r="B55">
-        <f>C54*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.6610781400623214</v>
       </c>
       <c r="C55">
-        <f>C54+B55</f>
+        <f t="shared" si="3"/>
         <v>167.76889214629446</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="2">
+      <c r="A56" s="1">
         <v>4.4166666666666696</v>
       </c>
       <c r="B56">
-        <f>C55*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.6776889214629447</v>
       </c>
       <c r="C56">
-        <f>C55+B56</f>
+        <f t="shared" si="3"/>
         <v>169.44658106775739</v>
       </c>
     </row>
@@ -1750,24 +1750,24 @@
         <v>4.5</v>
       </c>
       <c r="B57">
-        <f>C56*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.6944658106775741</v>
       </c>
       <c r="C57">
-        <f>C56+B57</f>
+        <f t="shared" si="3"/>
         <v>171.14104687843496</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="2">
+      <c r="A58" s="1">
         <v>4.5833333333333304</v>
       </c>
       <c r="B58">
-        <f>C57*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.7114104687843497</v>
       </c>
       <c r="C58">
-        <f>C57+B58</f>
+        <f t="shared" si="3"/>
         <v>172.85245734721931</v>
       </c>
     </row>
@@ -1776,24 +1776,24 @@
         <v>4.6666666666666696</v>
       </c>
       <c r="B59">
-        <f>C58*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.7285245734721932</v>
       </c>
       <c r="C59">
-        <f>C58+B59</f>
+        <f t="shared" si="3"/>
         <v>174.5809819206915</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="2">
+      <c r="A60" s="1">
         <v>4.75</v>
       </c>
       <c r="B60">
-        <f>C59*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.7458098192069151</v>
       </c>
       <c r="C60">
-        <f>C59+B60</f>
+        <f t="shared" si="3"/>
         <v>176.32679173989843</v>
       </c>
     </row>
@@ -1802,39 +1802,135 @@
         <v>4.8333333333333304</v>
       </c>
       <c r="B61">
-        <f>C60*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.7632679173989843</v>
       </c>
       <c r="C61">
-        <f>C60+B61</f>
+        <f t="shared" si="3"/>
         <v>178.09005965729742</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="2">
-        <v>4.9166666666666696</v>
+      <c r="A62" s="1">
+        <v>4.9166666666666599</v>
       </c>
       <c r="B62">
-        <f>C61*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.7809005965729743</v>
       </c>
       <c r="C62">
-        <f>C61+B62</f>
+        <f t="shared" ref="C62:C64" si="4">C61+B62</f>
         <v>179.87096025387038</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63">
-        <v>5</v>
+        <v>4.9999999999999902</v>
       </c>
       <c r="B63">
-        <f>C62*0.01</f>
+        <f t="shared" si="2"/>
         <v>1.7987096025387039</v>
       </c>
       <c r="C63">
-        <f>C62+B63</f>
+        <f t="shared" si="4"/>
         <v>181.66966985640909</v>
       </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="1"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="1"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="1"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="1"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="1"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="1"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="1"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="1"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" s="1"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" s="1"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" s="1"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" s="1"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" s="1"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" s="1"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" s="1"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" s="1"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" s="1"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" s="1"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" s="1"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" s="1"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" s="1"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" s="1"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A121" s="1"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>